<commit_message>
UPDATE documentos casos de pruebas y plan de pruebas
</commit_message>
<xml_diff>
--- a/Documentacion/PTP_JuanCarlosMIcanMuñoz_JhormanAlexanderCulmaHermosa_CasosDePrueba_y_Bugs_26092023.xlsx
+++ b/Documentacion/PTP_JuanCarlosMIcanMuñoz_JhormanAlexanderCulmaHermosa_CasosDePrueba_y_Bugs_26092023.xlsx
@@ -5,22 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\RETO\Senasoft2023Grupo4\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F439220B-E52C-4361-94F3-A370B4C30278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9EFBDC-E382-40F4-A5EF-7E4177E72A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Casos de prueba" sheetId="1" r:id="rId1"/>
+    <sheet name="Casos de prueba (Registro)" sheetId="1" r:id="rId1"/>
+    <sheet name="Casos de prueba (inicio sesión)" sheetId="3" r:id="rId2"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
   <si>
     <t>Id</t>
   </si>
@@ -49,30 +51,9 @@
     <t>Resultado esperado</t>
   </si>
   <si>
-    <t>BUGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Id Bug </t>
-  </si>
-  <si>
-    <t>Decripcion</t>
-  </si>
-  <si>
-    <t>Pasos a reproducir</t>
-  </si>
-  <si>
-    <t>Evidencias</t>
-  </si>
-  <si>
-    <t>Responsable a solucionar</t>
-  </si>
-  <si>
     <t>Validar que el registro ingreso correo electrónico valido.</t>
   </si>
   <si>
-    <t>Juan Carlos Mican Muñoz  y Jhorman Alexander culma Hermoza</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
@@ -134,6 +115,107 @@
   </si>
   <si>
     <t>REGISTRO</t>
+  </si>
+  <si>
+    <t>Juan Carlos Mican Muñoz  y Jhorman Alexander culma Hermosa</t>
+  </si>
+  <si>
+    <t>Validar que no permita el registro con una contraseña de menos de 10 caracteres y que no contenga una mayúscula y un número.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">que el usuario quiere crear su contraseña personal  </t>
+  </si>
+  <si>
+    <t>Ingrese una contraseña que no cumpla con los requerimientos solicitados</t>
+  </si>
+  <si>
+    <t>“La contraseña debe tener al menos 10 caracteres” , "La contraseña debe incluir al menos un número", "La contraseña debe incluir al menos una letra en mayúscula"</t>
+  </si>
+  <si>
+    <t>Se pudieron obtener cada una de las alertas esperadas</t>
+  </si>
+  <si>
+    <t>Se generarán 3 alertas, y no podra usar/crear esa contraseña</t>
+  </si>
+  <si>
+    <t>contra2023
+contraseñasegura
+contraseñasegura2023</t>
+  </si>
+  <si>
+    <t>Coincidencia de contraseñas</t>
+  </si>
+  <si>
+    <t>Validar requerimientos de contraseña.</t>
+  </si>
+  <si>
+    <t>Validar que el usuario sea advertido si las contraseñas no coinciden al momento del registro.</t>
+  </si>
+  <si>
+    <t>contraseña
+contraseñasegura2023
+confirmar contraseña
+contraseñasegura202</t>
+  </si>
+  <si>
+    <t xml:space="preserve">la confirma de manera errónea </t>
+  </si>
+  <si>
+    <t>que el usuario escribe su contraseña y la confirma</t>
+  </si>
+  <si>
+    <t>Se mostrará una alerta con el siguiente mensaje “Las contraseñas no coinciden. Inténtalo de nuevo.”</t>
+  </si>
+  <si>
+    <t>Las contraseñas no coinciden. Inténtalo de nuevo.</t>
+  </si>
+  <si>
+    <t>"Las contraseñas no coinciden. Inténtalo de nuevo."</t>
+  </si>
+  <si>
+    <t>Inicio de Sesión</t>
+  </si>
+  <si>
+    <t>Recuperar contraseña</t>
+  </si>
+  <si>
+    <t>Validar que exista una opción para recuperar mi contraseña.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> que el usuario olvido la contraseña, este quiere recuperar su cuenta</t>
+  </si>
+  <si>
+    <t>Deberá poder ver la opción de recuperar contraseña</t>
+  </si>
+  <si>
+    <t>Existe una opción llamada recuperar mi contraseña u ¿olvidaste tu contraseña?</t>
+  </si>
+  <si>
+    <t>No se encontró ese campo u otro relacionado a este</t>
+  </si>
+  <si>
+    <t>Validar que existe un registro con una dirección de email proporcionada por el usuario.</t>
+  </si>
+  <si>
+    <t>Validar si ya tiene una cuenta</t>
+  </si>
+  <si>
+    <t>example@correo.com</t>
+  </si>
+  <si>
+    <t>que el usuario no sabe si tiene ya creada una cuenta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">el ingrese su correo </t>
+  </si>
+  <si>
+    <t>El sistema validara si ya existe una cuenta con ese email o no</t>
+  </si>
+  <si>
+    <t>El sistema pedirá la contraseña para iniciar sesión</t>
+  </si>
+  <si>
+    <t>Se pidió la contraseña de la cuenta</t>
   </si>
 </sst>
 </file>
@@ -201,14 +283,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -233,18 +309,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -300,28 +373,70 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -337,38 +452,46 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}" name="Tabla1" displayName="Tabla1" ref="B3:O6" insertRowShift="1" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="B3:O6" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}" name="Tabla1" displayName="Tabla1" ref="B3:O7" insertRowShift="1" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+  <autoFilter ref="B3:O7" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{AF895A87-873C-49EB-A119-ADEB0B25950C}" name="Id" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{8F7EFCC1-486E-4994-8AD6-3BD68C4437CE}" name="Nombre" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{B6BC66A2-707D-46A7-9252-54B4842B51B8}" name="Responsable" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{9B9D85F8-DFC4-44E1-8542-6A148774F185}" name="Descripcion" dataDxfId="12"/>
-    <tableColumn id="5" xr3:uid="{A1C7689F-19AE-4CFF-9FC3-3E0CCA37702F}" name="Datos" dataDxfId="11"/>
-    <tableColumn id="16" xr3:uid="{FAE1E1BF-D927-480D-87E0-11800862A94E}" name="¿Automatizable?" dataDxfId="10"/>
-    <tableColumn id="8" xr3:uid="{B8D1966E-E2D0-4A94-989A-E2D3C5F98B62}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{BCAC0163-3B5B-4C70-AEA3-FB6EB8A3C54D}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="8"/>
-    <tableColumn id="10" xr3:uid="{B3BD0C4C-1476-4CE4-AF84-FAB02AFB1A2A}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{67B0E46A-7688-49E4-9D62-9BFEE6230D77}" name="Resultado esperado" dataDxfId="6"/>
-    <tableColumn id="12" xr3:uid="{AEDA80AD-F944-4FCA-9CAB-A942E633A2AD}" name="Resultado obtenido manualmente" dataDxfId="5"/>
-    <tableColumn id="6" xr3:uid="{FC4EB521-BDEB-4181-84E6-D282F4565798}" name="Resultado obtenido automatizado" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{DB11CD6D-6D50-4FEB-A36B-7D79FB369236}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{44658790-EBBB-4550-B0B1-9B6908EA5DDB}" name="Ciclo 2 Na" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{AF895A87-873C-49EB-A119-ADEB0B25950C}" name="Id" dataDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{8F7EFCC1-486E-4994-8AD6-3BD68C4437CE}" name="Nombre" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{B6BC66A2-707D-46A7-9252-54B4842B51B8}" name="Responsable" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{9B9D85F8-DFC4-44E1-8542-6A148774F185}" name="Descripcion" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{A1C7689F-19AE-4CFF-9FC3-3E0CCA37702F}" name="Datos" dataDxfId="25"/>
+    <tableColumn id="16" xr3:uid="{FAE1E1BF-D927-480D-87E0-11800862A94E}" name="¿Automatizable?" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{B8D1966E-E2D0-4A94-989A-E2D3C5F98B62}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{BCAC0163-3B5B-4C70-AEA3-FB6EB8A3C54D}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{B3BD0C4C-1476-4CE4-AF84-FAB02AFB1A2A}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{67B0E46A-7688-49E4-9D62-9BFEE6230D77}" name="Resultado esperado" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{AEDA80AD-F944-4FCA-9CAB-A942E633A2AD}" name="Resultado obtenido manualmente" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{FC4EB521-BDEB-4181-84E6-D282F4565798}" name="Resultado obtenido automatizado" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{DB11CD6D-6D50-4FEB-A36B-7D79FB369236}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="17"/>
+    <tableColumn id="14" xr3:uid="{44658790-EBBB-4550-B0B1-9B6908EA5DDB}" name="Ciclo 2 Na" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{F36325B5-0F2C-41D4-A0A4-A8685B8267F6}" name="Tabla2" displayName="Tabla2" ref="R4:W5" insertRow="1" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <autoFilter ref="R4:W5" xr:uid="{F36325B5-0F2C-41D4-A0A4-A8685B8267F6}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{6A3C8CA8-9D4C-4F2B-94B3-08621E2B1F4D}" name="Id Bug " dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{40DD1FE8-86B3-4588-BB1A-A3F74675848D}" name="Nombre" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{9CE72DF8-7B67-4E3A-BEE0-1C7268B9D7F2}" name="Decripcion" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{5B3F9488-6730-454C-A77B-E18F834CA054}" name="Pasos a reproducir" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{36688173-7D1F-4AD1-B1F5-16A5C2093FBC}" name="Evidencias" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{4C6570A4-163C-4BD2-99AB-F9B009FC8413}" name="Responsable a solucionar" dataDxfId="18"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91EA820B-BBC8-4258-A5F8-3A7798700EBB}" name="Tabla14" displayName="Tabla14" ref="B3:O5" insertRowShift="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="B3:O5" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{D6B56754-03D9-461F-AC4F-C35327C2183E}" name="Id" dataDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{0BF85DDA-853F-427E-B48E-4F0E40A91538}" name="Nombre" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{83BEA0E2-AC51-4B11-91E9-6469CABBC68D}" name="Responsable" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{A650FCD4-94EE-47A7-B661-27D59D2753A8}" name="Descripcion" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{DF684CCE-A777-46F0-B72D-1C062B7945C6}" name="Datos" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{218F28E1-9D6C-42CB-ABB3-CCBD66EECB44}" name="¿Automatizable?" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{1C8AA51D-5EE7-425C-9F71-DCA78A9069D6}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{1DA822E4-D0F5-48C2-AAE5-49AEDEBAFBAC}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{7A892534-37AF-4844-AEBE-3AC1E688EABF}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{D23BC59C-B577-4101-8CA9-EF609EDBE45E}" name="Resultado esperado" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{D28C4909-3E04-4EDF-8007-C11125A49C0F}" name="Resultado obtenido manualmente" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{F3DCF7C3-1CAC-4168-A226-D70A20EF46E5}" name="Resultado obtenido automatizado" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{129491C9-D93B-4844-B0A1-AB9EBAB4BADF}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{F863331A-0ECD-4CEF-BE8F-421DCD4787A1}" name="Ciclo 2 Na" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -671,213 +794,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W6"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView topLeftCell="L7" zoomScale="94" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="6"/>
-    <col min="2" max="2" width="9.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="56.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="47.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="49.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="31.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="31.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="31.28515625" style="6" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:23">
-      <c r="H1" s="10" t="s">
+    <row r="1" spans="2:15">
+      <c r="H1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="3" spans="2:15" ht="30">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="75">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="75">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="105">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="10"/>
+      <c r="K6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="2:23" ht="30">
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
+    <row r="7" spans="2:15" ht="75">
+      <c r="B7" s="1">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="2:23" ht="75">
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M4" s="3"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="T4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="U4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="W4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="2:23" ht="75">
-      <c r="B5" s="3">
-        <v>2</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="M5" s="3"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-      <c r="U5" s="1"/>
-      <c r="V5" s="1"/>
-      <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="2:23">
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="R3:W3"/>
+  <mergeCells count="1">
     <mergeCell ref="H1:I1"/>
   </mergeCells>
   <hyperlinks>
@@ -885,9 +1036,192 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId3"/>
-    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CEBCCA-16A6-49F6-860C-EB26F898AD42}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="2" max="2" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="56.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="47.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="31.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15">
+      <c r="H1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="8"/>
+    </row>
+    <row r="3" spans="2:15" ht="30">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="60">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="M4" s="1"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="75">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M5" s="1"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1" xr:uid="{D7F66BBC-CAEE-44BE-B315-2CF030571ACA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3382C1-2BF3-48C7-A27B-FC5FA3603097}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Bugs y casos de pruebas Añadidos
</commit_message>
<xml_diff>
--- a/Documentacion/PTP_JuanCarlosMIcanMuñoz_JhormanAlexanderCulmaHermosa_CasosDePrueba_y_Bugs_26092023.xlsx
+++ b/Documentacion/PTP_JuanCarlosMIcanMuñoz_JhormanAlexanderCulmaHermosa_CasosDePrueba_y_Bugs_26092023.xlsx
@@ -5,24 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\RETO\Senasoft2023Grupo4\Documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\SenaSoft\Senasoft2023Grupo4\Documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9EFBDC-E382-40F4-A5EF-7E4177E72A0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1B9EEA-75F0-450B-A0D2-9E3A97F63FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Casos de prueba (Registro)" sheetId="1" r:id="rId1"/>
     <sheet name="Casos de prueba (inicio sesión)" sheetId="3" r:id="rId2"/>
-    <sheet name="Hoja1" sheetId="2" r:id="rId3"/>
+    <sheet name="C P(BarranavegUtilidades)" sheetId="2" r:id="rId3"/>
+    <sheet name="CP(Barra Navegacion Paginas Se)" sheetId="4" r:id="rId4"/>
+    <sheet name="Bugs" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191028"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="136">
   <si>
     <t>Id</t>
   </si>
@@ -216,13 +218,232 @@
   </si>
   <si>
     <t>Se pidió la contraseña de la cuenta</t>
+  </si>
+  <si>
+    <t> Validar que no tengo una cuenta creada en Booking.com.</t>
+  </si>
+  <si>
+    <t>Validar que el usuario actual no cuente con una cuenta de usuario en Booking.com</t>
+  </si>
+  <si>
+    <t>PePe10pepxx@gmail.com</t>
+  </si>
+  <si>
+    <t>Dado que el usuario esta en la pagina de inicio de session</t>
+  </si>
+  <si>
+    <t>Cuando Ingresa el correo electronico en el campo del formulario</t>
+  </si>
+  <si>
+    <t>Entonces El usuario vera en pantalla el titulo "Crea una contraseña"</t>
+  </si>
+  <si>
+    <t>Titulo en pantalla "Crea una contraseña"</t>
+  </si>
+  <si>
+    <t>"Crea una contraseña"</t>
+  </si>
+  <si>
+    <t>Se validará que el elemento ancla “Booking.com” re direccione a la página principal.</t>
+  </si>
+  <si>
+    <t>Validar que el elemento de ancla en el aplicativo y mas especificamente en el componente de navegacion de utilidades fucione y redireccione al usuario a la pagina de inicio</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Dado que el usuario esta en la pagina de inicio de la aplicación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando el usuario da click en un boton de navegacion "Vuelos" </t>
+  </si>
+  <si>
+    <t>Entonces EL usuario vera en pantalla el titulo de pagina "Compara y reserva vuelos fácilmente"</t>
+  </si>
+  <si>
+    <t>Titulo en pantalla "Compara y reserva vuelos fácilmente"</t>
+  </si>
+  <si>
+    <t>"Compara y reserva vuelos fácilmente"</t>
+  </si>
+  <si>
+    <t>Se validará que al modificar la divisa el divisa cambie en la barra del menú.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que al modificar la divisa el tipo de divisa cambie al deseado y sea mostrado en la pantalla </t>
+  </si>
+  <si>
+    <t>USD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando el usuario da click en la opcion de cambio de divisa y selecciona "USD" </t>
+  </si>
+  <si>
+    <t>Entonces El usuario Vera en la barra de navegacion de utilidades las palabras "USD"</t>
+  </si>
+  <si>
+    <t>Palabras en navegacion de "USD"</t>
+  </si>
+  <si>
+    <t>Palabras obtenidas en la barra de navegacion "USD"</t>
+  </si>
+  <si>
+    <t>Se validará que al modificar  el idioma se vean los cambios de idioma.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validar que al modificar el idioma el idioma de la pagina cambie al deseado y sea mostrado en la pantalla </t>
+  </si>
+  <si>
+    <t>English(US)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando el usuario da click en la opcion de cambio de idioma y selecciona "English(US)" </t>
+  </si>
+  <si>
+    <t>Entonces El usuario Vera en la barra de navegacion de utilidades las palabras "English(US)"</t>
+  </si>
+  <si>
+    <t>Palabras en navegacion de "English(US)"</t>
+  </si>
+  <si>
+    <t>Palabras obtenidas en la barra de navegacion "English(US)"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entonces el usuario puede ver el titulo principal de la pagina seleccionada </t>
+  </si>
+  <si>
+    <t>Barra de navegacion de utilidades</t>
+  </si>
+  <si>
+    <t>Barra de navegacion de paginas de servicios</t>
+  </si>
+  <si>
+    <t>BUGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Id Bug </t>
+  </si>
+  <si>
+    <t>Decripcion</t>
+  </si>
+  <si>
+    <t>Pasos a reproducir</t>
+  </si>
+  <si>
+    <t>Evidencias</t>
+  </si>
+  <si>
+    <t>Responsable a solucionar</t>
+  </si>
+  <si>
+    <t>Falta el hipervinculo de recuperar cuenta</t>
+  </si>
+  <si>
+    <t>No se encuentra la funcionalidad ni el elemento de recuperar la cuenta en el aplicativo en la pagina de inicio de session</t>
+  </si>
+  <si>
+    <t>Entrar a la pagina de registro del aplicativo de Booking.com y evidenciar el formulario expuesto</t>
+  </si>
+  <si>
+    <t>Equipo de desarrollo encargado de Booking.com</t>
+  </si>
+  <si>
+    <t>Errores en la reprensentacion de idiomas en el aplicativo Booking.com</t>
+  </si>
+  <si>
+    <t>Error en las banderas de los paises que representan los idiomas por ejemplo el de español, argentina, mexico.</t>
+  </si>
+  <si>
+    <t>Entrar al aplicativo Booking.com y en el navegador de utilidades y interactuar con la funcionalidad de cambio de idioma y encontraras los errores de representacion de idiomas y dialecto</t>
+  </si>
+  <si>
+    <t>Error uno de escritura</t>
+  </si>
+  <si>
+    <t>Error de escritura en el footer con la traduccion de la siguiente oracion al español "Bed and breakfasts" por que esta en ingles y no esta en español estando yo en la pagina con idioma en español.</t>
+  </si>
+  <si>
+    <t>Entrar al aplicativo Booking.com y en la zona del footer leer y encontrar las palabras descritas previamente en la fila.</t>
+  </si>
+  <si>
+    <t>Error dos de escritura</t>
+  </si>
+  <si>
+    <t>Error de escritura en el footer con la traduccion de la siguiente oracion al español "Traveller Review Awards" por que esta en ingles y no esta en español estando yo en la pagina con idioma en español.</t>
+  </si>
+  <si>
+    <t>Error tres de escritura</t>
+  </si>
+  <si>
+    <t>Error de escritura en el footer con la traduccion de la siguiente oracion al español "Careers" por que esta en ingles y no esta en español estando yo en la pagina con idioma en español.</t>
+  </si>
+  <si>
+    <t>Se validará que la opcion del menu de paginas de servicios "Alojamiento" redireccione a la página solicitada y esta sea mostrada en pantalla.</t>
+  </si>
+  <si>
+    <t>Se validará que la opcion del menu de paginas de servicios "Vuelos" redireccione a la página solicitada y esta sea mostrada en pantalla.</t>
+  </si>
+  <si>
+    <t>Se validará que la opcion del menu de paginas de servicios "Alquiler de coches" redireccione a la página solicitada y esta sea mostrada en pantalla.</t>
+  </si>
+  <si>
+    <t>Se validará que la opcion del menu de paginas de servicios "Atracciones turísticas" redireccione a la página solicitada y esta sea mostrada en pantalla.</t>
+  </si>
+  <si>
+    <t>Se validará que la opcion del menu de paginas de servicios "Taxis aeropuerto" redireccione a la página solicitada y esta sea mostrada en pantalla.</t>
+  </si>
+  <si>
+    <t>Validar que el menu de paginas de servicios redireccione correctamente a las paginas correspondiente de "Alojamiento"</t>
+  </si>
+  <si>
+    <t>Validar que el menu de paginas de servicios redireccione correctamente a las paginas correspondiente de "Vuelos"</t>
+  </si>
+  <si>
+    <t>Validar que el menu de paginas de servicios redireccione correctamente a las paginas correspondiente de "Alquiler de coches"</t>
+  </si>
+  <si>
+    <t>Validar que el menu de paginas de servicios redireccione correctamente a las paginas correspondiente de "Atracciones turísticas"</t>
+  </si>
+  <si>
+    <t>Validar que el menu de paginas de servicios redireccione correctamente a las paginas correspondiente de "Taxis aeropuerto"</t>
+  </si>
+  <si>
+    <t>Cuando el usuario da click en el botones de navegacion del menu de paginas de servicio para ver la pagina "Alojamiento"</t>
+  </si>
+  <si>
+    <t>Cuando el usuario da click en el botones de navegacion del menu de paginas de servicio para ver la pagina "Vuelos"</t>
+  </si>
+  <si>
+    <t>Cuando el usuario da click en el botones de navegacion del menu de paginas de servicio para ver la pagina "Alquiler de coches"</t>
+  </si>
+  <si>
+    <t>Cuando el usuario da click en el botones de navegacion del menu de paginas de servicio para ver la pagina "Atracciones turísticas"</t>
+  </si>
+  <si>
+    <t>Cuando el usuario da click en el botones de navegacion del menu de paginas de servicio para ver la pagina "Taxis aeropuerto"</t>
+  </si>
+  <si>
+    <t>Titulo de la pagina "Encuentra tu próxima estancia"</t>
+  </si>
+  <si>
+    <t>Titulo de la pagina "Compara y reserva vuelos fácilmente"</t>
+  </si>
+  <si>
+    <t>Titulo de la pagina " Alquiler de coches para cualquier tipo de viaje"</t>
+  </si>
+  <si>
+    <t>Titulo de la pagina " Reserva un taxi desde o al aeropuerto"</t>
+  </si>
+  <si>
+    <t>Titulo de la pagina " Atracciones, actividades y experiencias"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -243,8 +464,31 @@
       <color rgb="FF1A1A1A"/>
       <name val="Var(--DO_NOT_USE_bui_large_font"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,12 +513,71 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4472C4"/>
+        <bgColor rgb="FF4472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9E1F2"/>
+        <bgColor rgb="FFD9E1F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -283,7 +586,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -309,7 +612,49 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -317,7 +662,364 @@
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="62">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD9E1F2"/>
+          <bgColor rgb="FFD9E1F2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4472C4"/>
+          <bgColor rgb="FF4472C4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4"/>
+          <bgColor theme="4"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -451,47 +1153,363 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>273599</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>147153</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3989457</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2037820</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCEBE4C8-BAF9-32A3-C874-52DB2FB50413}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6734034" y="1113457"/>
+          <a:ext cx="3715858" cy="1890667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>220871</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1021521</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4050137</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>2112065</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagen 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2CF1DB9-7939-4E60-EA0C-29111667DEBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6681306" y="4375978"/>
+          <a:ext cx="3829266" cy="1090544"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>96631</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1035326</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3724668</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>1711739</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF899BC7-F72F-7884-8B88-52B7F2528434}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6557066" y="7440543"/>
+          <a:ext cx="3628037" cy="676413"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>138044</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1049132</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>4148916</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1776104</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagen 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5C7D15A-69C0-EA05-E895-FE78F5CBDC9B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6598479" y="10311849"/>
+          <a:ext cx="4010872" cy="726972"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>828262</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>814455</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>3478696</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1731914</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagen 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{731C9E1A-C6E8-42F0-E3AC-92D8FB6F9322}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7288697" y="13321194"/>
+          <a:ext cx="2650434" cy="917459"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}" name="Tabla1" displayName="Tabla1" ref="B3:O7" insertRowShift="1" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}" name="Tabla1" displayName="Tabla1" ref="B3:O7" insertRowShift="1" totalsRowShown="0" headerRowDxfId="61" dataDxfId="60">
   <autoFilter ref="B3:O7" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{AF895A87-873C-49EB-A119-ADEB0B25950C}" name="Id" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{8F7EFCC1-486E-4994-8AD6-3BD68C4437CE}" name="Nombre" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{B6BC66A2-707D-46A7-9252-54B4842B51B8}" name="Responsable" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{9B9D85F8-DFC4-44E1-8542-6A148774F185}" name="Descripcion" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{A1C7689F-19AE-4CFF-9FC3-3E0CCA37702F}" name="Datos" dataDxfId="25"/>
-    <tableColumn id="16" xr3:uid="{FAE1E1BF-D927-480D-87E0-11800862A94E}" name="¿Automatizable?" dataDxfId="24"/>
-    <tableColumn id="8" xr3:uid="{B8D1966E-E2D0-4A94-989A-E2D3C5F98B62}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="23"/>
-    <tableColumn id="9" xr3:uid="{BCAC0163-3B5B-4C70-AEA3-FB6EB8A3C54D}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="22"/>
-    <tableColumn id="10" xr3:uid="{B3BD0C4C-1476-4CE4-AF84-FAB02AFB1A2A}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="21"/>
-    <tableColumn id="11" xr3:uid="{67B0E46A-7688-49E4-9D62-9BFEE6230D77}" name="Resultado esperado" dataDxfId="20"/>
-    <tableColumn id="12" xr3:uid="{AEDA80AD-F944-4FCA-9CAB-A942E633A2AD}" name="Resultado obtenido manualmente" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{FC4EB521-BDEB-4181-84E6-D282F4565798}" name="Resultado obtenido automatizado" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{DB11CD6D-6D50-4FEB-A36B-7D79FB369236}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="17"/>
-    <tableColumn id="14" xr3:uid="{44658790-EBBB-4550-B0B1-9B6908EA5DDB}" name="Ciclo 2 Na" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{AF895A87-873C-49EB-A119-ADEB0B25950C}" name="Id" dataDxfId="59"/>
+    <tableColumn id="2" xr3:uid="{8F7EFCC1-486E-4994-8AD6-3BD68C4437CE}" name="Nombre" dataDxfId="58"/>
+    <tableColumn id="3" xr3:uid="{B6BC66A2-707D-46A7-9252-54B4842B51B8}" name="Responsable" dataDxfId="57"/>
+    <tableColumn id="4" xr3:uid="{9B9D85F8-DFC4-44E1-8542-6A148774F185}" name="Descripcion" dataDxfId="56"/>
+    <tableColumn id="5" xr3:uid="{A1C7689F-19AE-4CFF-9FC3-3E0CCA37702F}" name="Datos" dataDxfId="55"/>
+    <tableColumn id="16" xr3:uid="{FAE1E1BF-D927-480D-87E0-11800862A94E}" name="¿Automatizable?" dataDxfId="54"/>
+    <tableColumn id="8" xr3:uid="{B8D1966E-E2D0-4A94-989A-E2D3C5F98B62}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="53"/>
+    <tableColumn id="9" xr3:uid="{BCAC0163-3B5B-4C70-AEA3-FB6EB8A3C54D}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="52"/>
+    <tableColumn id="10" xr3:uid="{B3BD0C4C-1476-4CE4-AF84-FAB02AFB1A2A}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="51"/>
+    <tableColumn id="11" xr3:uid="{67B0E46A-7688-49E4-9D62-9BFEE6230D77}" name="Resultado esperado" dataDxfId="50"/>
+    <tableColumn id="12" xr3:uid="{AEDA80AD-F944-4FCA-9CAB-A942E633A2AD}" name="Resultado obtenido manualmente" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{FC4EB521-BDEB-4181-84E6-D282F4565798}" name="Resultado obtenido automatizado" dataDxfId="48"/>
+    <tableColumn id="13" xr3:uid="{DB11CD6D-6D50-4FEB-A36B-7D79FB369236}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="47"/>
+    <tableColumn id="14" xr3:uid="{44658790-EBBB-4550-B0B1-9B6908EA5DDB}" name="Ciclo 2 Na" dataDxfId="46"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91EA820B-BBC8-4258-A5F8-3A7798700EBB}" name="Tabla14" displayName="Tabla14" ref="B3:O5" insertRowShift="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="B3:O5" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{91EA820B-BBC8-4258-A5F8-3A7798700EBB}" name="Tabla14" displayName="Tabla14" ref="B3:O6" insertRowShift="1" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44">
+  <autoFilter ref="B3:O6" xr:uid="{59E4E730-58B4-4D9B-96F4-7068CDEC5D8F}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{D6B56754-03D9-461F-AC4F-C35327C2183E}" name="Id" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{0BF85DDA-853F-427E-B48E-4F0E40A91538}" name="Nombre" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{83BEA0E2-AC51-4B11-91E9-6469CABBC68D}" name="Responsable" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A650FCD4-94EE-47A7-B661-27D59D2753A8}" name="Descripcion" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{DF684CCE-A777-46F0-B72D-1C062B7945C6}" name="Datos" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{218F28E1-9D6C-42CB-ABB3-CCBD66EECB44}" name="¿Automatizable?" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{1C8AA51D-5EE7-425C-9F71-DCA78A9069D6}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{1DA822E4-D0F5-48C2-AAE5-49AEDEBAFBAC}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{7A892534-37AF-4844-AEBE-3AC1E688EABF}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{D23BC59C-B577-4101-8CA9-EF609EDBE45E}" name="Resultado esperado" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{D28C4909-3E04-4EDF-8007-C11125A49C0F}" name="Resultado obtenido manualmente" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{F3DCF7C3-1CAC-4168-A226-D70A20EF46E5}" name="Resultado obtenido automatizado" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{129491C9-D93B-4844-B0A1-AB9EBAB4BADF}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="1"/>
-    <tableColumn id="14" xr3:uid="{F863331A-0ECD-4CEF-BE8F-421DCD4787A1}" name="Ciclo 2 Na" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D6B56754-03D9-461F-AC4F-C35327C2183E}" name="Id" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{0BF85DDA-853F-427E-B48E-4F0E40A91538}" name="Nombre" dataDxfId="42"/>
+    <tableColumn id="3" xr3:uid="{83BEA0E2-AC51-4B11-91E9-6469CABBC68D}" name="Responsable" dataDxfId="41"/>
+    <tableColumn id="4" xr3:uid="{A650FCD4-94EE-47A7-B661-27D59D2753A8}" name="Descripcion" dataDxfId="40"/>
+    <tableColumn id="5" xr3:uid="{DF684CCE-A777-46F0-B72D-1C062B7945C6}" name="Datos" dataDxfId="39"/>
+    <tableColumn id="16" xr3:uid="{218F28E1-9D6C-42CB-ABB3-CCBD66EECB44}" name="¿Automatizable?" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{1C8AA51D-5EE7-425C-9F71-DCA78A9069D6}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{1DA822E4-D0F5-48C2-AAE5-49AEDEBAFBAC}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{7A892534-37AF-4844-AEBE-3AC1E688EABF}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{D23BC59C-B577-4101-8CA9-EF609EDBE45E}" name="Resultado esperado" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{D28C4909-3E04-4EDF-8007-C11125A49C0F}" name="Resultado obtenido manualmente" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{F3DCF7C3-1CAC-4168-A226-D70A20EF46E5}" name="Resultado obtenido automatizado" dataDxfId="32"/>
+    <tableColumn id="13" xr3:uid="{129491C9-D93B-4844-B0A1-AB9EBAB4BADF}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="31"/>
+    <tableColumn id="14" xr3:uid="{F863331A-0ECD-4CEF-BE8F-421DCD4787A1}" name="Ciclo 2 Na" dataDxfId="30"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{1ADEF6C0-1242-4E83-9B38-CB71507EEDF2}" name="Tabla2" displayName="Tabla2" ref="B3:O6" totalsRowShown="0" headerRowDxfId="24" headerRowBorderDxfId="28" tableBorderDxfId="29" totalsRowBorderDxfId="27">
+  <autoFilter ref="B3:O6" xr:uid="{1ADEF6C0-1242-4E83-9B38-CB71507EEDF2}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{BE1F664F-1924-4F8B-9EFD-9DC2AB4A0856}" name="Id"/>
+    <tableColumn id="2" xr3:uid="{12C8D864-B4E5-4891-A1D8-A3EFC3A244FF}" name="Nombre"/>
+    <tableColumn id="3" xr3:uid="{3A77D9B5-16DB-4049-BBE3-1D90E83DF3EA}" name="Responsable"/>
+    <tableColumn id="4" xr3:uid="{307A95FC-704C-4C21-85DB-E20474A66F6B}" name="Descripcion"/>
+    <tableColumn id="5" xr3:uid="{25317A1A-B002-4B8A-BB26-11AB6ED9AEA7}" name="Datos"/>
+    <tableColumn id="6" xr3:uid="{CEA6717D-E299-46F5-929B-2A525C2CA498}" name="¿Automatizable?"/>
+    <tableColumn id="7" xr3:uid="{49C98253-4921-424C-8F3C-24FF32A543E5}" name="Dado &lt;Una situacion o estado&gt;"/>
+    <tableColumn id="8" xr3:uid="{62F582F8-AD85-49CB-954D-110DB7998ED4}" name="Cuando &lt;realizar alguna accion&gt;"/>
+    <tableColumn id="9" xr3:uid="{A9F87F4D-FA91-4ABE-85C7-812002CDA86D}" name="Entonces&lt;lograr algun resultado&gt;"/>
+    <tableColumn id="10" xr3:uid="{109A4EFB-495F-4C92-A1DF-21CC002F6653}" name="Resultado esperado"/>
+    <tableColumn id="11" xr3:uid="{73B05CE7-84BC-47A2-82D8-29506693A0CF}" name="Resultado obtenido manualmente"/>
+    <tableColumn id="12" xr3:uid="{8B67D6B5-8AA1-450F-88EF-BB94443637FA}" name="Resultado obtenido automatizado"/>
+    <tableColumn id="13" xr3:uid="{72D7EB4A-424E-4FCA-8A6C-EB641FBF061A}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="26"/>
+    <tableColumn id="14" xr3:uid="{602FC90C-8EED-4464-B3FC-165EBF3746FA}" name="Ciclo 2 Na" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{993375AC-213D-4634-A19F-7CF90412CB53}" name="Tabla15" displayName="Tabla15" ref="B3:O8" insertRowShift="1" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+  <autoFilter ref="B3:O8" xr:uid="{993375AC-213D-4634-A19F-7CF90412CB53}"/>
+  <tableColumns count="14">
+    <tableColumn id="1" xr3:uid="{570BF129-306C-4A4C-9933-380B9D0BC862}" name="Id" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{876CA9D5-3D88-4DE5-81FF-CC5EF1070FFD}" name="Nombre" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{8530F711-8608-4D49-8E5A-EB3273610C0F}" name="Responsable" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{7584B6CC-C6CE-4059-9CC0-B248D4E40B41}" name="Descripcion" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{46DF13B3-ADF1-4DB1-80C1-639068572DDE}" name="Datos" dataDxfId="17"/>
+    <tableColumn id="16" xr3:uid="{DAAF289F-8441-4860-A183-9E0353874A19}" name="¿Automatizable?" dataDxfId="16"/>
+    <tableColumn id="8" xr3:uid="{FD3179A3-6E5E-45C9-AEA8-53DC5C455EF0}" name="Dado &lt;Una situacion o estado&gt;" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{083CA385-3232-4D5B-88B5-D571A07A01F1}" name="Cuando &lt;realizar alguna accion&gt;" dataDxfId="14"/>
+    <tableColumn id="10" xr3:uid="{36F70616-8379-42BF-81D2-246D7C9FD98A}" name="Entonces&lt;lograr algun resultado&gt;" dataDxfId="13"/>
+    <tableColumn id="11" xr3:uid="{DD57A4F8-9252-420B-9FE3-522819D1D58D}" name="Resultado esperado" dataDxfId="12"/>
+    <tableColumn id="12" xr3:uid="{47B8D010-063A-4B25-8348-6509EC75F49A}" name="Resultado obtenido manualmente" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{8C195910-F446-4295-B0AF-A302D13A8C46}" name="Resultado obtenido automatizado" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{10F6A3A0-9687-44F0-90E5-110702EAD22F}" name="Ciclo 1 fecha 26/09/2023" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{703A1E66-995B-4CEC-AACF-4E0FBBE80A5F}" name="Ciclo 2 Na" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{EB169E1A-D5DC-4656-8BE7-9B0DA1FBFBBF}" name="Tabla3" displayName="Tabla3" ref="C4:H9" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
+  <autoFilter ref="C4:H9" xr:uid="{EB169E1A-D5DC-4656-8BE7-9B0DA1FBFBBF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{FDA343DE-CD54-43A9-9853-A0B6061AAA96}" name="Id Bug " dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{F3B1E432-938E-4E6B-949D-245BFDFBACF1}" name="Nombre" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{4A7FA4BD-ECA0-45E8-AA9C-D88CD1B0BD36}" name="Decripcion" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{EBE48029-570C-4AC7-9E84-B48EBF0F88F2}" name="Pasos a reproducir" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{76799E10-0C6F-44A4-8E69-EF80BD1E6F3E}" name="Evidencias" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{502D46D7-7F89-4C03-9FC3-A0D4E5898521}" name="Responsable a solucionar" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -796,11 +1814,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="L7" zoomScale="94" workbookViewId="0">
+    <sheetView topLeftCell="A6" zoomScale="94" workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -819,13 +1837,13 @@
     <col min="15" max="15" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H1" s="8" t="s">
         <v>30</v>
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="3" spans="2:15" ht="30">
+    <row r="3" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -869,7 +1887,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="75">
+    <row r="4" spans="2:15" ht="75" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -909,7 +1927,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="75">
+    <row r="5" spans="2:15" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -949,7 +1967,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="2:15" ht="105">
+    <row r="6" spans="2:15" ht="105" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -984,11 +2002,11 @@
         <v>36</v>
       </c>
       <c r="N6" s="6"/>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="2:15" ht="75">
+    <row r="7" spans="2:15" ht="75" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -1023,7 +2041,7 @@
         <v>46</v>
       </c>
       <c r="N7" s="6"/>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1044,13 +2062,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77CEBCCA-16A6-49F6-860C-EB26F898AD42}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="94" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5:N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="4"/>
     <col min="2" max="2" width="9.42578125" style="4" bestFit="1" customWidth="1"/>
@@ -1069,13 +2087,13 @@
     <col min="15" max="15" width="15.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15">
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
       <c r="H1" s="8" t="s">
         <v>48</v>
       </c>
       <c r="I1" s="8"/>
     </row>
-    <row r="3" spans="2:15" ht="30">
+    <row r="3" spans="2:15" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -1119,7 +2137,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="60">
+    <row r="4" spans="2:15" ht="60" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -1159,7 +2177,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="75">
+    <row r="5" spans="2:15" ht="75" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -1196,6 +2214,45 @@
       <c r="M5" s="1"/>
       <c r="N5" s="6"/>
       <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1205,23 +2262,662 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1" xr:uid="{D7F66BBC-CAEE-44BE-B315-2CF030571ACA}"/>
+    <hyperlink ref="F6" r:id="rId2" xr:uid="{9CFBEEB8-34B8-46CD-8555-7CD15903212D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA3382C1-2BF3-48C7-A27B-FC5FA3603097}">
-  <dimension ref="A1"/>
+  <dimension ref="B1:O6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" zoomScale="91" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="35.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="F1" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+    </row>
+    <row r="3" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="195" x14ac:dyDescent="0.25">
+      <c r="B4" s="11">
+        <v>1</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" s="13"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="105" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="M5" s="12"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="120" x14ac:dyDescent="0.25">
+      <c r="B6" s="16">
+        <v>3</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="L6" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC0D34E-ECE8-4E99-A650-378A286BB5A9}">
+  <dimension ref="B1:O8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="69" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="G1" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+    </row>
+    <row r="3" spans="2:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="M4" s="4"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="135" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>2</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="M5" s="4"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M6" s="4"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15" ht="165" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15" ht="150" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>5</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59C907A5-635D-459F-A152-D0D8EDC3FDFB}">
+  <dimension ref="C3:H9"/>
+  <sheetViews>
+    <sheetView topLeftCell="A9" zoomScale="69" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="21" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
+      <c r="G3" s="21"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="3:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="G4" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="H4" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" ht="188.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="23">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="240" x14ac:dyDescent="0.25">
+      <c r="C6" s="23">
+        <v>2</v>
+      </c>
+      <c r="D6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="F6" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="C7" s="23">
+        <v>3</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="255" x14ac:dyDescent="0.25">
+      <c r="C8" s="23">
+        <v>4</v>
+      </c>
+      <c r="D8" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="225" x14ac:dyDescent="0.25">
+      <c r="C9" s="23">
+        <v>5</v>
+      </c>
+      <c r="D9" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23" t="s">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:H3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>